<commit_message>
add version tab in the master spreadsheet
</commit_message>
<xml_diff>
--- a/master_spreadsheet.xlsx
+++ b/master_spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/genomics-invoicing-25-26Summer-Test-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/genomics-invoicing-25-26Summer-Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D39EA4C-906E-CF48-88CE-31EA662C8923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9B16EF-C7A8-AC48-A9AD-2F26DEF325DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="16080" activeTab="2" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="2160" yWindow="580" windowWidth="25600" windowHeight="16080" activeTab="5" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List" sheetId="8" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Config" sheetId="4" r:id="rId3"/>
     <sheet name="Discount" sheetId="10" r:id="rId4"/>
     <sheet name="Surcharge Editing Page" sheetId="11" r:id="rId5"/>
+    <sheet name="Info" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Combined Price List'!$A$1:$G$18</definedName>
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="106">
   <si>
     <t>Product Code</t>
   </si>
@@ -404,6 +405,33 @@
   </si>
   <si>
     <t>Please use the "Surcharge editing page" for all surcharge updates. To ensure the accuracy of system calculations, please avoid modifying this Config page directly. Thank you for your cooperation!</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>v0.6</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>GitHub Repo</t>
+  </si>
+  <si>
+    <t>https://github.com/yiliyayaya/genomics-invoicing-25-26Summer-Test</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Genomics Invoicing Project (25-26 Summer)</t>
+  </si>
+  <si>
+    <t>This master spreadsheet stores the key data used in the Shiny application</t>
   </si>
 </sst>
 </file>
@@ -415,7 +443,7 @@
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,6 +610,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -606,10 +656,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -678,8 +729,29 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1055,7 +1127,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1676,7 +1748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D55C99-92A7-4BC5-9E4D-8387E6974F28}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
+    <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2113,16 +2185,80 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B677D6A2-0063-084E-86E1-5492E421B735}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.749992370372631"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="38">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{2912F4FD-196E-2343-A039-791D9F5CD5E4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c">
@@ -2132,6 +2268,15 @@
     <Notes xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2404,20 +2549,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
     <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Revert "add version tab in the master spreadsheet"
</commit_message>
<xml_diff>
--- a/master_spreadsheet.xlsx
+++ b/master_spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/genomics-invoicing-25-26Summer-Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilia/Desktop/genomics-invoicing-25-26Summer-Test-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9B16EF-C7A8-AC48-A9AD-2F26DEF325DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D39EA4C-906E-CF48-88CE-31EA662C8923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="580" windowWidth="25600" windowHeight="16080" activeTab="5" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="16080" activeTab="2" xr2:uid="{44EEA75D-67FD-4678-9465-A167448191E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Price List" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Config" sheetId="4" r:id="rId3"/>
     <sheet name="Discount" sheetId="10" r:id="rId4"/>
     <sheet name="Surcharge Editing Page" sheetId="11" r:id="rId5"/>
-    <sheet name="Info" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Combined Price List'!$A$1:$G$18</definedName>
@@ -114,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="97">
   <si>
     <t>Product Code</t>
   </si>
@@ -405,33 +404,6 @@
   </si>
   <si>
     <t>Please use the "Surcharge editing page" for all surcharge updates. To ensure the accuracy of system calculations, please avoid modifying this Config page directly. Thank you for your cooperation!</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>v0.6</t>
-  </si>
-  <si>
-    <t>Last Updated</t>
-  </si>
-  <si>
-    <t>GitHub Repo</t>
-  </si>
-  <si>
-    <t>https://github.com/yiliyayaya/genomics-invoicing-25-26Summer-Test</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>Genomics Invoicing Project (25-26 Summer)</t>
-  </si>
-  <si>
-    <t>This master spreadsheet stores the key data used in the Shiny application</t>
   </si>
 </sst>
 </file>
@@ -443,7 +415,7 @@
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,28 +582,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -656,11 +606,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -729,29 +678,8 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1127,7 +1055,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1748,7 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D55C99-92A7-4BC5-9E4D-8387E6974F28}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2185,80 +2113,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B677D6A2-0063-084E-86E1-5492E421B735}">
-  <sheetPr>
-    <tabColor theme="3" tint="0.749992370372631"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="59.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="38">
-        <v>46037</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{2912F4FD-196E-2343-A039-791D9F5CD5E4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c">
@@ -2268,15 +2132,6 @@
     <Notes xmlns="17163bdb-27fe-447c-a7bb-3ea6416b971c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2549,20 +2404,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343B393C-CAC2-4750-ACA8-00CCC9C377F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="17163bdb-27fe-447c-a7bb-3ea6416b971c"/>
     <ds:schemaRef ds:uri="451c1f4f-a267-451c-a3af-09c2fa4691f1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8371111F-EFF7-47C6-8985-0F43994E666C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>